<commit_message>
Added some examples, and non-csvkit pure bash examples that are helpful.
</commit_message>
<xml_diff>
--- a/dat/xlsx_mtcars.xlsx
+++ b/dat/xlsx_mtcars.xlsx
@@ -158,16 +158,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -188,6 +180,19 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -231,13 +236,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -573,1273 +579,1276 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>21</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>160</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>110</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>3.9</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>2.62</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>16.46</v>
       </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1</v>
-      </c>
-      <c r="K2" s="1">
-        <v>4</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>21</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>160</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>110</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>3.9</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>2.875</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>17.02</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>22.8</v>
       </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
         <v>108</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>93</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>3.85</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>2.3199999999999998</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>18.61</v>
       </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>4</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4</v>
+      </c>
+      <c r="L4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>21.4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>258</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>110</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>3.08</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="3">
         <v>3.2149999999999999</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="3">
         <v>19.440000000000001</v>
       </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>3</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>18.7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>360</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>175</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>3.15</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="3">
         <v>3.44</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="3">
         <v>17.02</v>
       </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1">
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>18.100000000000001</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>225</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>105</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>2.76</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
         <v>3.46</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="3">
         <v>20.22</v>
       </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>14.3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>8</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>360</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>245</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>3.21</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>3.57</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>15.84</v>
       </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>24.4</v>
       </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
         <v>146.69999999999999</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>62</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>3.69</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>3.19</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="3">
         <v>20</v>
       </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>4</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>22.8</v>
       </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
         <v>140.80000000000001</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>95</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>3.92</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>3.15</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="3">
         <v>22.9</v>
       </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>4</v>
-      </c>
-      <c r="L10" s="1">
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>19.2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>6</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>167.6</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>123</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>3.92</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="3">
         <v>3.44</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="3">
         <v>18.3</v>
       </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>4</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="L11" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>17.8</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>6</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>167.6</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>123</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>3.92</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>3.44</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="3">
         <v>18.899999999999999</v>
       </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>4</v>
-      </c>
-      <c r="L12" s="1">
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>8</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>275.8</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>180</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>3.07</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>4.07</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>3</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>17.3</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>8</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>275.8</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <v>180</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <v>3.07</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
         <v>3.73</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="3">
         <v>17.600000000000001</v>
       </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>3</v>
-      </c>
-      <c r="L14" s="1">
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>15.2</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>8</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>275.8</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>180</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>3.07</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="3">
         <v>3.78</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="3">
         <v>18</v>
       </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>3</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>10.4</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>472</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>205</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>2.93</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
         <v>5.25</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="3">
         <v>17.98</v>
       </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>3</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3</v>
+      </c>
+      <c r="L16" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>10.4</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>460</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <v>215</v>
       </c>
-      <c r="F17" s="1">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
         <v>5.4240000000000004</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="3">
         <v>17.82</v>
       </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>3</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>14.7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>8</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="3">
         <v>440</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="3">
         <v>230</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="3">
         <v>3.23</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="3">
         <v>5.3449999999999998</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="3">
         <v>17.420000000000002</v>
       </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
-        <v>3</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>32.4</v>
       </c>
-      <c r="C19" s="1">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="3">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
         <v>78.7</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="3">
         <v>66</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="3">
         <v>4.08</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="3">
         <v>19.47</v>
       </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>4</v>
+      </c>
+      <c r="L19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>30.4</v>
       </c>
-      <c r="C20" s="1">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3">
         <v>75.7</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>52</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>4.93</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="3">
         <v>1.615</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="3">
         <v>18.52</v>
       </c>
-      <c r="I20" s="1">
-        <v>1</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20" s="1">
-        <v>4</v>
-      </c>
-      <c r="L20" s="1">
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
+        <v>4</v>
+      </c>
+      <c r="L20" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>33.9</v>
       </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3">
         <v>71.099999999999994</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>65</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>4.22</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="3">
         <v>1.835</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="3">
         <v>19.899999999999999</v>
       </c>
-      <c r="I21" s="1">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1</v>
-      </c>
-      <c r="K21" s="1">
-        <v>4</v>
-      </c>
-      <c r="L21" s="1">
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>4</v>
+      </c>
+      <c r="L21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>21.5</v>
       </c>
-      <c r="C22" s="1">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3">
         <v>120.1</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <v>97</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="3">
         <v>3.7</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
         <v>2.4649999999999999</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="3">
         <v>20.010000000000002</v>
       </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>3</v>
-      </c>
-      <c r="L22" s="1">
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>15.5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>8</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="3">
         <v>318</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <v>150</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="3">
         <v>2.76</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="3">
         <v>3.52</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="3">
         <v>16.87</v>
       </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <v>3</v>
-      </c>
-      <c r="L23" s="1">
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="3">
         <v>15.2</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="3">
         <v>8</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="3">
         <v>304</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="3">
         <v>150</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="3">
         <v>3.15</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="3">
         <v>3.4350000000000001</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="3">
         <v>17.3</v>
       </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
-        <v>3</v>
-      </c>
-      <c r="L24" s="1">
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>3</v>
+      </c>
+      <c r="L24" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="3">
         <v>13.3</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <v>8</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="3">
         <v>350</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="3">
         <v>245</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="3">
         <v>3.73</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="3">
         <v>3.84</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="3">
         <v>15.41</v>
       </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1">
-        <v>3</v>
-      </c>
-      <c r="L25" s="1">
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>3</v>
+      </c>
+      <c r="L25" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>19.2</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <v>8</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="3">
         <v>400</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="3">
         <v>175</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="3">
         <v>3.08</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
         <v>3.8450000000000002</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="3">
         <v>17.05</v>
       </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1">
-        <v>3</v>
-      </c>
-      <c r="L26" s="1">
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>3</v>
+      </c>
+      <c r="L26" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="3">
         <v>27.3</v>
       </c>
-      <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3">
         <v>79</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="3">
         <v>66</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="3">
         <v>4.08</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="3">
         <v>1.9350000000000001</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="3">
         <v>18.899999999999999</v>
       </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1">
-        <v>4</v>
-      </c>
-      <c r="L27" s="1">
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4</v>
+      </c>
+      <c r="L27" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>26</v>
       </c>
-      <c r="C28" s="1">
-        <v>4</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3">
         <v>120.3</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="3">
         <v>91</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="3">
         <v>4.43</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="3">
         <v>2.14</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="3">
         <v>16.7</v>
       </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1</v>
-      </c>
-      <c r="K28" s="1">
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3">
         <v>5</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L28" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="3">
         <v>30.4</v>
       </c>
-      <c r="C29" s="1">
-        <v>4</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="3">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3">
         <v>95.1</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="3">
         <v>113</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29" s="3">
         <v>3.77</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="3">
         <v>1.5129999999999999</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="3">
         <v>16.899999999999999</v>
       </c>
-      <c r="I29" s="1">
-        <v>1</v>
-      </c>
-      <c r="J29" s="1">
-        <v>1</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
         <v>5</v>
       </c>
-      <c r="L29" s="1">
+      <c r="L29" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="3">
         <v>15.8</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="3">
         <v>8</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="3">
         <v>351</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="3">
         <v>264</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="3">
         <v>4.22</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="3">
         <v>3.17</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="3">
         <v>14.5</v>
       </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
-        <v>1</v>
-      </c>
-      <c r="K30" s="1">
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
         <v>5</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L30" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="3">
         <v>19.7</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="3">
         <v>6</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="3">
         <v>145</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="3">
         <v>175</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="3">
         <v>3.62</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="3">
         <v>2.77</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="3">
         <v>15.5</v>
       </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1">
-        <v>1</v>
-      </c>
-      <c r="K31" s="1">
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
         <v>5</v>
       </c>
-      <c r="L31" s="1">
+      <c r="L31" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="3">
         <v>15</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="3">
         <v>8</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="3">
         <v>301</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="3">
         <v>335</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="3">
         <v>3.54</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="3">
         <v>3.57</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="3">
         <v>14.6</v>
       </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
-      <c r="J32" s="1">
-        <v>1</v>
-      </c>
-      <c r="K32" s="1">
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3">
         <v>5</v>
       </c>
-      <c r="L32" s="1">
+      <c r="L32" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="3">
         <v>21.4</v>
       </c>
-      <c r="C33" s="1">
-        <v>4</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3">
         <v>121</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="3">
         <v>109</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="3">
         <v>4.1100000000000003</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="3">
         <v>2.78</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="3">
         <v>18.600000000000001</v>
       </c>
-      <c r="I33" s="1">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1">
-        <v>1</v>
-      </c>
-      <c r="K33" s="1">
-        <v>4</v>
-      </c>
-      <c r="L33" s="1">
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>4</v>
+      </c>
+      <c r="L33" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>